<commit_message>
Refactor & added features
- Subject top
- Overall Top
</commit_message>
<xml_diff>
--- a/cse.xlsx
+++ b/cse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Heman\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Venu\Documents\GitHub\GradeR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A972D36-F511-499C-8B2D-B6DFAEF1DBED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8104EB6D-B735-41EF-A5C5-57A9BF5829DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -842,19 +842,19 @@
     </r>
   </si>
   <si>
-    <t>GRADE</t>
+    <t>Htno</t>
   </si>
   <si>
-    <t>CREDIT</t>
+    <t>Subcode</t>
   </si>
   <si>
-    <t>SUBJECT</t>
+    <t>Subname</t>
   </si>
   <si>
-    <t>CODE</t>
+    <t>Grade</t>
   </si>
   <si>
-    <t>ROLL</t>
+    <t>Credits</t>
   </si>
 </sst>
 </file>
@@ -1276,35 +1276,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E512"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" customWidth="1"/>
+    <col min="3" max="3" width="62.5" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
         <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1321,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1338,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1355,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1372,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1389,7 +1391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1406,7 +1408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1423,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1440,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1457,7 +1459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1474,7 +1476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1491,7 +1493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1508,7 +1510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1525,7 +1527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -1542,7 +1544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1559,7 +1561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1576,7 +1578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1593,7 +1595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -1610,7 +1612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1627,7 +1629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -1644,7 +1646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1661,7 +1663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
@@ -1678,7 +1680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1695,7 +1697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
@@ -1712,7 +1714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1729,7 +1731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1746,7 +1748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1763,7 +1765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
@@ -1780,7 +1782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -1797,7 +1799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>26</v>
       </c>
@@ -1814,7 +1816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -1831,7 +1833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>26</v>
       </c>
@@ -1848,7 +1850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -1865,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>27</v>
       </c>
@@ -1882,7 +1884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
@@ -1899,7 +1901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>27</v>
       </c>
@@ -1916,7 +1918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>27</v>
       </c>
@@ -1933,7 +1935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>27</v>
       </c>
@@ -1950,7 +1952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>27</v>
       </c>
@@ -1967,7 +1969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>27</v>
       </c>
@@ -1984,7 +1986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>28</v>
       </c>
@@ -2001,7 +2003,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>28</v>
       </c>
@@ -2018,7 +2020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
@@ -2035,7 +2037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>28</v>
       </c>
@@ -2052,7 +2054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>28</v>
       </c>
@@ -2069,7 +2071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>28</v>
       </c>
@@ -2086,7 +2088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>28</v>
       </c>
@@ -2103,7 +2105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>28</v>
       </c>
@@ -2120,7 +2122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>29</v>
       </c>
@@ -2137,7 +2139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>29</v>
       </c>
@@ -2154,7 +2156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
@@ -2171,7 +2173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>29</v>
       </c>
@@ -2188,7 +2190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>29</v>
       </c>
@@ -2205,7 +2207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>29</v>
       </c>
@@ -2222,7 +2224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>29</v>
       </c>
@@ -2239,7 +2241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>29</v>
       </c>
@@ -2256,7 +2258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>30</v>
       </c>
@@ -2273,7 +2275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>30</v>
       </c>
@@ -2290,7 +2292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>30</v>
       </c>
@@ -2307,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>30</v>
       </c>
@@ -2324,7 +2326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>30</v>
       </c>
@@ -2341,7 +2343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>30</v>
       </c>
@@ -2358,7 +2360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>30</v>
       </c>
@@ -2375,7 +2377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>30</v>
       </c>
@@ -2392,7 +2394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>31</v>
       </c>
@@ -2409,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>31</v>
       </c>
@@ -2426,7 +2428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>31</v>
       </c>
@@ -2443,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>31</v>
       </c>
@@ -2460,7 +2462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>31</v>
       </c>
@@ -2477,7 +2479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>31</v>
       </c>
@@ -2494,7 +2496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>31</v>
       </c>
@@ -2511,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>31</v>
       </c>
@@ -2528,7 +2530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>32</v>
       </c>
@@ -2545,7 +2547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>32</v>
       </c>
@@ -2562,7 +2564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>32</v>
       </c>
@@ -2579,7 +2581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>32</v>
       </c>
@@ -2596,7 +2598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>32</v>
       </c>
@@ -2613,7 +2615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>32</v>
       </c>
@@ -2630,7 +2632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>32</v>
       </c>
@@ -2647,7 +2649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>32</v>
       </c>
@@ -2664,7 +2666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>33</v>
       </c>
@@ -2681,7 +2683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>33</v>
       </c>
@@ -2698,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>33</v>
       </c>
@@ -2715,7 +2717,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>33</v>
       </c>
@@ -2732,7 +2734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>33</v>
       </c>
@@ -2749,7 +2751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>33</v>
       </c>
@@ -2766,7 +2768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>33</v>
       </c>
@@ -2783,7 +2785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>33</v>
       </c>
@@ -2800,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>34</v>
       </c>
@@ -2817,7 +2819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>34</v>
       </c>
@@ -2834,7 +2836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>34</v>
       </c>
@@ -2851,7 +2853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>34</v>
       </c>
@@ -2868,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>34</v>
       </c>
@@ -2885,7 +2887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>34</v>
       </c>
@@ -2902,7 +2904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>34</v>
       </c>
@@ -2919,7 +2921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>34</v>
       </c>
@@ -2936,7 +2938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>35</v>
       </c>
@@ -2953,7 +2955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>35</v>
       </c>
@@ -2970,7 +2972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>35</v>
       </c>
@@ -2987,7 +2989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>35</v>
       </c>
@@ -3004,7 +3006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>35</v>
       </c>
@@ -3021,7 +3023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>35</v>
       </c>
@@ -3038,7 +3040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>35</v>
       </c>
@@ -3055,7 +3057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>35</v>
       </c>
@@ -3072,7 +3074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>36</v>
       </c>
@@ -3089,7 +3091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>36</v>
       </c>
@@ -3106,7 +3108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>36</v>
       </c>
@@ -3123,7 +3125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>36</v>
       </c>
@@ -3140,7 +3142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>36</v>
       </c>
@@ -3157,7 +3159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>36</v>
       </c>
@@ -3174,7 +3176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>36</v>
       </c>
@@ -3191,7 +3193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>36</v>
       </c>
@@ -3208,7 +3210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>37</v>
       </c>
@@ -3225,7 +3227,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>37</v>
       </c>
@@ -3242,7 +3244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>37</v>
       </c>
@@ -3259,7 +3261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>37</v>
       </c>
@@ -3276,7 +3278,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>37</v>
       </c>
@@ -3293,7 +3295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>37</v>
       </c>
@@ -3310,7 +3312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>37</v>
       </c>
@@ -3327,7 +3329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>37</v>
       </c>
@@ -3344,7 +3346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>38</v>
       </c>
@@ -3361,7 +3363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>38</v>
       </c>
@@ -3378,7 +3380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>38</v>
       </c>
@@ -3395,7 +3397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>38</v>
       </c>
@@ -3412,7 +3414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>38</v>
       </c>
@@ -3429,7 +3431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>38</v>
       </c>
@@ -3446,7 +3448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>38</v>
       </c>
@@ -3463,7 +3465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>38</v>
       </c>
@@ -3480,7 +3482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>39</v>
       </c>
@@ -3497,7 +3499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>39</v>
       </c>
@@ -3514,7 +3516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>39</v>
       </c>
@@ -3531,7 +3533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>39</v>
       </c>
@@ -3548,7 +3550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>39</v>
       </c>
@@ -3565,7 +3567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>39</v>
       </c>
@@ -3582,7 +3584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>39</v>
       </c>
@@ -3599,7 +3601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>39</v>
       </c>
@@ -3616,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>40</v>
       </c>
@@ -3633,7 +3635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>40</v>
       </c>
@@ -3650,7 +3652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>40</v>
       </c>
@@ -3667,7 +3669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>40</v>
       </c>
@@ -3684,7 +3686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>40</v>
       </c>
@@ -3701,7 +3703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>40</v>
       </c>
@@ -3718,7 +3720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>40</v>
       </c>
@@ -3735,7 +3737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>40</v>
       </c>
@@ -3752,7 +3754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>41</v>
       </c>
@@ -3769,7 +3771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>41</v>
       </c>
@@ -3786,7 +3788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>41</v>
       </c>
@@ -3803,7 +3805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>41</v>
       </c>
@@ -3820,7 +3822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>41</v>
       </c>
@@ -3837,7 +3839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>41</v>
       </c>
@@ -3854,7 +3856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>41</v>
       </c>
@@ -3871,7 +3873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>41</v>
       </c>
@@ -3888,7 +3890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>42</v>
       </c>
@@ -3905,7 +3907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>42</v>
       </c>
@@ -3922,7 +3924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>42</v>
       </c>
@@ -3939,7 +3941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>42</v>
       </c>
@@ -3956,7 +3958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>42</v>
       </c>
@@ -3973,7 +3975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>42</v>
       </c>
@@ -3990,7 +3992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>42</v>
       </c>
@@ -4007,7 +4009,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>42</v>
       </c>
@@ -4024,7 +4026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>43</v>
       </c>
@@ -4041,7 +4043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>43</v>
       </c>
@@ -4058,7 +4060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>43</v>
       </c>
@@ -4075,7 +4077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>43</v>
       </c>
@@ -4092,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>43</v>
       </c>
@@ -4109,7 +4111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>43</v>
       </c>
@@ -4126,7 +4128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>43</v>
       </c>
@@ -4143,7 +4145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>43</v>
       </c>
@@ -4160,7 +4162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>44</v>
       </c>
@@ -4177,7 +4179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>44</v>
       </c>
@@ -4194,7 +4196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>44</v>
       </c>
@@ -4211,7 +4213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>44</v>
       </c>
@@ -4228,7 +4230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>44</v>
       </c>
@@ -4245,7 +4247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>44</v>
       </c>
@@ -4262,7 +4264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>44</v>
       </c>
@@ -4279,7 +4281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>44</v>
       </c>
@@ -4296,7 +4298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>45</v>
       </c>
@@ -4313,7 +4315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>45</v>
       </c>
@@ -4330,7 +4332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>45</v>
       </c>
@@ -4347,7 +4349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>45</v>
       </c>
@@ -4364,7 +4366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>45</v>
       </c>
@@ -4381,7 +4383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
         <v>45</v>
       </c>
@@ -4398,7 +4400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>45</v>
       </c>
@@ -4415,7 +4417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>45</v>
       </c>
@@ -4432,7 +4434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>46</v>
       </c>
@@ -4449,7 +4451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
         <v>46</v>
       </c>
@@ -4466,7 +4468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>46</v>
       </c>
@@ -4483,7 +4485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
         <v>46</v>
       </c>
@@ -4500,7 +4502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>46</v>
       </c>
@@ -4517,7 +4519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
         <v>46</v>
       </c>
@@ -4534,7 +4536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>46</v>
       </c>
@@ -4551,7 +4553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
         <v>46</v>
       </c>
@@ -4568,7 +4570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>47</v>
       </c>
@@ -4585,7 +4587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>47</v>
       </c>
@@ -4602,7 +4604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>47</v>
       </c>
@@ -4619,7 +4621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>47</v>
       </c>
@@ -4636,7 +4638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>47</v>
       </c>
@@ -4653,7 +4655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>47</v>
       </c>
@@ -4670,7 +4672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>47</v>
       </c>
@@ -4687,7 +4689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
         <v>47</v>
       </c>
@@ -4704,7 +4706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>48</v>
       </c>
@@ -4721,7 +4723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>48</v>
       </c>
@@ -4738,7 +4740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>48</v>
       </c>
@@ -4755,7 +4757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>48</v>
       </c>
@@ -4772,7 +4774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>48</v>
       </c>
@@ -4789,7 +4791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
         <v>48</v>
       </c>
@@ -4806,7 +4808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>48</v>
       </c>
@@ -4823,7 +4825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
         <v>48</v>
       </c>
@@ -4840,7 +4842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>49</v>
       </c>
@@ -4857,7 +4859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
         <v>49</v>
       </c>
@@ -4874,7 +4876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>49</v>
       </c>
@@ -4891,7 +4893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
         <v>49</v>
       </c>
@@ -4908,7 +4910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>49</v>
       </c>
@@ -4925,7 +4927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
         <v>49</v>
       </c>
@@ -4942,7 +4944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>49</v>
       </c>
@@ -4959,7 +4961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
         <v>49</v>
       </c>
@@ -4976,7 +4978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>50</v>
       </c>
@@ -4993,7 +4995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
         <v>50</v>
       </c>
@@ -5010,7 +5012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>50</v>
       </c>
@@ -5027,7 +5029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
         <v>50</v>
       </c>
@@ -5044,7 +5046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>50</v>
       </c>
@@ -5061,7 +5063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
         <v>50</v>
       </c>
@@ -5078,7 +5080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>50</v>
       </c>
@@ -5095,7 +5097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
         <v>50</v>
       </c>
@@ -5112,7 +5114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>51</v>
       </c>
@@ -5129,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
         <v>51</v>
       </c>
@@ -5146,7 +5148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>51</v>
       </c>
@@ -5163,7 +5165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
         <v>51</v>
       </c>
@@ -5180,7 +5182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>51</v>
       </c>
@@ -5197,7 +5199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
         <v>51</v>
       </c>
@@ -5214,7 +5216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>51</v>
       </c>
@@ -5231,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
         <v>51</v>
       </c>
@@ -5248,7 +5250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>52</v>
       </c>
@@ -5265,7 +5267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
         <v>52</v>
       </c>
@@ -5282,7 +5284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="236" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>52</v>
       </c>
@@ -5299,7 +5301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
         <v>52</v>
       </c>
@@ -5316,7 +5318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>52</v>
       </c>
@@ -5333,7 +5335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
         <v>52</v>
       </c>
@@ -5350,7 +5352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>52</v>
       </c>
@@ -5367,7 +5369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
         <v>52</v>
       </c>
@@ -5384,7 +5386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="242" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>53</v>
       </c>
@@ -5401,7 +5403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="243" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
         <v>53</v>
       </c>
@@ -5418,7 +5420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>53</v>
       </c>
@@ -5435,7 +5437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="245" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
         <v>53</v>
       </c>
@@ -5452,7 +5454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>53</v>
       </c>
@@ -5469,7 +5471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
         <v>53</v>
       </c>
@@ -5486,7 +5488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>53</v>
       </c>
@@ -5503,7 +5505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="249" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>53</v>
       </c>
@@ -5520,7 +5522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>54</v>
       </c>
@@ -5537,7 +5539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="251" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
         <v>54</v>
       </c>
@@ -5554,7 +5556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="252" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>54</v>
       </c>
@@ -5571,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
         <v>54</v>
       </c>
@@ -5588,7 +5590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="254" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>54</v>
       </c>
@@ -5605,7 +5607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>54</v>
       </c>
@@ -5622,7 +5624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>54</v>
       </c>
@@ -5639,7 +5641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="257" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>54</v>
       </c>
@@ -5656,7 +5658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:5" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>55</v>
       </c>
@@ -5673,7 +5675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
         <v>55</v>
       </c>
@@ -5690,7 +5692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="260" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>55</v>
       </c>
@@ -5707,7 +5709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
         <v>55</v>
       </c>
@@ -5724,7 +5726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>55</v>
       </c>
@@ -5741,7 +5743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
         <v>55</v>
       </c>
@@ -5758,7 +5760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>55</v>
       </c>
@@ -5775,7 +5777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>55</v>
       </c>
@@ -5792,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>56</v>
       </c>
@@ -5809,7 +5811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="267" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>56</v>
       </c>
@@ -5826,7 +5828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="268" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>56</v>
       </c>
@@ -5843,7 +5845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>56</v>
       </c>
@@ -5860,7 +5862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>56</v>
       </c>
@@ -5877,7 +5879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="271" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>56</v>
       </c>
@@ -5894,7 +5896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>56</v>
       </c>
@@ -5911,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>56</v>
       </c>
@@ -5928,7 +5930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="274" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>57</v>
       </c>
@@ -5945,7 +5947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="275" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
         <v>57</v>
       </c>
@@ -5962,7 +5964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="276" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>57</v>
       </c>
@@ -5979,7 +5981,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="277" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>57</v>
       </c>
@@ -5996,7 +5998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="278" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>57</v>
       </c>
@@ -6013,7 +6015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
         <v>57</v>
       </c>
@@ -6030,7 +6032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>57</v>
       </c>
@@ -6047,7 +6049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
         <v>57</v>
       </c>
@@ -6064,7 +6066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="282" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>58</v>
       </c>
@@ -6081,7 +6083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="283" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
         <v>58</v>
       </c>
@@ -6098,7 +6100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="284" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
         <v>58</v>
       </c>
@@ -6115,7 +6117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
         <v>58</v>
       </c>
@@ -6132,7 +6134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="286" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
         <v>58</v>
       </c>
@@ -6149,7 +6151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
         <v>58</v>
       </c>
@@ -6166,7 +6168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>58</v>
       </c>
@@ -6183,7 +6185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
         <v>58</v>
       </c>
@@ -6200,7 +6202,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="290" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
         <v>59</v>
       </c>
@@ -6217,7 +6219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="291" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
         <v>59</v>
       </c>
@@ -6234,7 +6236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="292" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>59</v>
       </c>
@@ -6251,7 +6253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="293" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
         <v>59</v>
       </c>
@@ -6268,7 +6270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="294" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
         <v>59</v>
       </c>
@@ -6285,7 +6287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
         <v>59</v>
       </c>
@@ -6302,7 +6304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="296" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
         <v>59</v>
       </c>
@@ -6319,7 +6321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="297" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
         <v>59</v>
       </c>
@@ -6336,7 +6338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
         <v>60</v>
       </c>
@@ -6353,7 +6355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="299" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
         <v>60</v>
       </c>
@@ -6370,7 +6372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="300" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>60</v>
       </c>
@@ -6387,7 +6389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="301" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
         <v>60</v>
       </c>
@@ -6404,7 +6406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="302" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>60</v>
       </c>
@@ -6421,7 +6423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="303" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
         <v>60</v>
       </c>
@@ -6438,7 +6440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
         <v>60</v>
       </c>
@@ -6455,7 +6457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="305" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
         <v>60</v>
       </c>
@@ -6472,7 +6474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="306" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
         <v>61</v>
       </c>
@@ -6489,7 +6491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="307" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
         <v>61</v>
       </c>
@@ -6506,7 +6508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>61</v>
       </c>
@@ -6523,7 +6525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:5" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
         <v>61</v>
       </c>
@@ -6540,7 +6542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>61</v>
       </c>
@@ -6557,7 +6559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
         <v>61</v>
       </c>
@@ -6574,7 +6576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
         <v>61</v>
       </c>
@@ -6591,7 +6593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
         <v>61</v>
       </c>
@@ -6608,7 +6610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="314" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
         <v>62</v>
       </c>
@@ -6625,7 +6627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="315" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
         <v>62</v>
       </c>
@@ -6642,7 +6644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="316" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" s="1" t="s">
         <v>62</v>
       </c>
@@ -6659,7 +6661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="317" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="3" t="s">
         <v>62</v>
       </c>
@@ -6676,7 +6678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="318" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
         <v>62</v>
       </c>
@@ -6693,7 +6695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
         <v>62</v>
       </c>
@@ -6710,7 +6712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
         <v>62</v>
       </c>
@@ -6727,7 +6729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="321" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="s">
         <v>62</v>
       </c>
@@ -6744,7 +6746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="322" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
         <v>63</v>
       </c>
@@ -6761,7 +6763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
         <v>63</v>
       </c>
@@ -6778,7 +6780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="324" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>63</v>
       </c>
@@ -6795,7 +6797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="325" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="s">
         <v>63</v>
       </c>
@@ -6812,7 +6814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="326" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>63</v>
       </c>
@@ -6829,7 +6831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="327" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" s="3" t="s">
         <v>63</v>
       </c>
@@ -6846,7 +6848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="328" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
         <v>63</v>
       </c>
@@ -6863,7 +6865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="329" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="3" t="s">
         <v>63</v>
       </c>
@@ -6880,7 +6882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="330" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
         <v>64</v>
       </c>
@@ -6897,7 +6899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="331" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="s">
         <v>64</v>
       </c>
@@ -6914,7 +6916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="332" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" s="1" t="s">
         <v>64</v>
       </c>
@@ -6931,7 +6933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="333" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
         <v>64</v>
       </c>
@@ -6948,7 +6950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="334" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
         <v>64</v>
       </c>
@@ -6965,7 +6967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="335" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="s">
         <v>64</v>
       </c>
@@ -6982,7 +6984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" s="1" t="s">
         <v>64</v>
       </c>
@@ -6999,7 +7001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="337" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="s">
         <v>64</v>
       </c>
@@ -7016,7 +7018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="338" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
         <v>65</v>
       </c>
@@ -7033,7 +7035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="339" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
         <v>65</v>
       </c>
@@ -7050,7 +7052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="340" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
         <v>65</v>
       </c>
@@ -7067,7 +7069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="341" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
         <v>65</v>
       </c>
@@ -7084,7 +7086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="342" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
         <v>65</v>
       </c>
@@ -7101,7 +7103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="343" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">
         <v>65</v>
       </c>
@@ -7118,7 +7120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A344" s="1" t="s">
         <v>65</v>
       </c>
@@ -7135,7 +7137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="345" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="s">
         <v>65</v>
       </c>
@@ -7152,7 +7154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="346" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="1" t="s">
         <v>66</v>
       </c>
@@ -7169,7 +7171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="347" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="3" t="s">
         <v>66</v>
       </c>
@@ -7186,7 +7188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" s="1" t="s">
         <v>66</v>
       </c>
@@ -7203,7 +7205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="349" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" s="3" t="s">
         <v>66</v>
       </c>
@@ -7220,7 +7222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="350" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
         <v>66</v>
       </c>
@@ -7237,7 +7239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A351" s="3" t="s">
         <v>66</v>
       </c>
@@ -7254,7 +7256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="352" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>66</v>
       </c>
@@ -7271,7 +7273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="353" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="s">
         <v>66</v>
       </c>
@@ -7288,7 +7290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="354" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>67</v>
       </c>
@@ -7305,7 +7307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="355" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="s">
         <v>67</v>
       </c>
@@ -7322,7 +7324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="356" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>67</v>
       </c>
@@ -7339,7 +7341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="357" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A357" s="3" t="s">
         <v>67</v>
       </c>
@@ -7356,7 +7358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="358" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
         <v>67</v>
       </c>
@@ -7373,7 +7375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="359" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A359" s="3" t="s">
         <v>67</v>
       </c>
@@ -7390,7 +7392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="360" spans="1:5" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
         <v>67</v>
       </c>
@@ -7407,7 +7409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="361" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A361" s="3" t="s">
         <v>67</v>
       </c>
@@ -7424,7 +7426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="s">
         <v>68</v>
       </c>
@@ -7441,7 +7443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="363" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A363" s="3" t="s">
         <v>68</v>
       </c>
@@ -7458,7 +7460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="364" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
         <v>68</v>
       </c>
@@ -7475,7 +7477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="365" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A365" s="3" t="s">
         <v>68</v>
       </c>
@@ -7492,7 +7494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="366" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
         <v>68</v>
       </c>
@@ -7509,7 +7511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="367" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A367" s="3" t="s">
         <v>68</v>
       </c>
@@ -7526,7 +7528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="368" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A368" s="1" t="s">
         <v>68</v>
       </c>
@@ -7543,7 +7545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="369" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A369" s="3" t="s">
         <v>68</v>
       </c>
@@ -7560,7 +7562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="370" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A370" s="1" t="s">
         <v>69</v>
       </c>
@@ -7577,7 +7579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="371" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A371" s="3" t="s">
         <v>69</v>
       </c>
@@ -7594,7 +7596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="372" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A372" s="1" t="s">
         <v>69</v>
       </c>
@@ -7611,7 +7613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="373" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A373" s="3" t="s">
         <v>69</v>
       </c>
@@ -7628,7 +7630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="374" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
         <v>69</v>
       </c>
@@ -7645,7 +7647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="375" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A375" s="3" t="s">
         <v>69</v>
       </c>
@@ -7662,7 +7664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="376" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A376" s="1" t="s">
         <v>69</v>
       </c>
@@ -7679,7 +7681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="377" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A377" s="3" t="s">
         <v>69</v>
       </c>
@@ -7696,7 +7698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="378" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A378" s="1" t="s">
         <v>70</v>
       </c>
@@ -7713,7 +7715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="379" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A379" s="3" t="s">
         <v>70</v>
       </c>
@@ -7730,7 +7732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="380" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A380" s="1" t="s">
         <v>70</v>
       </c>
@@ -7747,7 +7749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="381" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A381" s="3" t="s">
         <v>70</v>
       </c>
@@ -7764,7 +7766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="382" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A382" s="1" t="s">
         <v>70</v>
       </c>
@@ -7781,7 +7783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="383" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A383" s="3" t="s">
         <v>70</v>
       </c>
@@ -7798,7 +7800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="384" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A384" s="1" t="s">
         <v>70</v>
       </c>
@@ -7815,7 +7817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="385" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A385" s="3" t="s">
         <v>70</v>
       </c>
@@ -7832,7 +7834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="386" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A386" s="1" t="s">
         <v>71</v>
       </c>
@@ -7849,7 +7851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="387" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A387" s="3" t="s">
         <v>71</v>
       </c>
@@ -7866,7 +7868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="388" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A388" s="1" t="s">
         <v>71</v>
       </c>
@@ -7883,7 +7885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="389" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A389" s="3" t="s">
         <v>71</v>
       </c>
@@ -7900,7 +7902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="390" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A390" s="1" t="s">
         <v>71</v>
       </c>
@@ -7917,7 +7919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="391" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A391" s="3" t="s">
         <v>71</v>
       </c>
@@ -7934,7 +7936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="392" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A392" s="1" t="s">
         <v>71</v>
       </c>
@@ -7951,7 +7953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="393" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A393" s="3" t="s">
         <v>71</v>
       </c>
@@ -7968,7 +7970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="394" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A394" s="1" t="s">
         <v>72</v>
       </c>
@@ -7985,7 +7987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="395" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A395" s="3" t="s">
         <v>72</v>
       </c>
@@ -8002,7 +8004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="396" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
         <v>72</v>
       </c>
@@ -8019,7 +8021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="397" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A397" s="3" t="s">
         <v>72</v>
       </c>
@@ -8036,7 +8038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="398" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A398" s="1" t="s">
         <v>72</v>
       </c>
@@ -8053,7 +8055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="399" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A399" s="3" t="s">
         <v>72</v>
       </c>
@@ -8070,7 +8072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="400" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A400" s="1" t="s">
         <v>72</v>
       </c>
@@ -8087,7 +8089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="401" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A401" s="3" t="s">
         <v>72</v>
       </c>
@@ -8104,7 +8106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="402" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A402" s="1" t="s">
         <v>73</v>
       </c>
@@ -8121,7 +8123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="403" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A403" s="3" t="s">
         <v>73</v>
       </c>
@@ -8138,7 +8140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="404" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A404" s="1" t="s">
         <v>73</v>
       </c>
@@ -8155,7 +8157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="405" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A405" s="3" t="s">
         <v>73</v>
       </c>
@@ -8172,7 +8174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="406" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
         <v>73</v>
       </c>
@@ -8189,7 +8191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="407" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A407" s="3" t="s">
         <v>73</v>
       </c>
@@ -8206,7 +8208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="408" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
         <v>73</v>
       </c>
@@ -8223,7 +8225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="409" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A409" s="3" t="s">
         <v>73</v>
       </c>
@@ -8240,7 +8242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="410" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A410" s="1" t="s">
         <v>74</v>
       </c>
@@ -8257,7 +8259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="411" spans="1:5" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A411" s="3" t="s">
         <v>74</v>
       </c>
@@ -8274,7 +8276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="412" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A412" s="1" t="s">
         <v>74</v>
       </c>
@@ -8291,7 +8293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A413" s="3" t="s">
         <v>74</v>
       </c>
@@ -8308,7 +8310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="414" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A414" s="1" t="s">
         <v>74</v>
       </c>
@@ -8325,7 +8327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="415" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A415" s="3" t="s">
         <v>74</v>
       </c>
@@ -8342,7 +8344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="416" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A416" s="1" t="s">
         <v>74</v>
       </c>
@@ -8359,7 +8361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="417" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A417" s="3" t="s">
         <v>74</v>
       </c>
@@ -8376,7 +8378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A418" s="1" t="s">
         <v>75</v>
       </c>
@@ -8393,7 +8395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="419" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A419" s="3" t="s">
         <v>75</v>
       </c>
@@ -8410,7 +8412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="420" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A420" s="1" t="s">
         <v>75</v>
       </c>
@@ -8427,7 +8429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="421" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A421" s="3" t="s">
         <v>75</v>
       </c>
@@ -8444,7 +8446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A422" s="1" t="s">
         <v>75</v>
       </c>
@@ -8461,7 +8463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="423" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A423" s="3" t="s">
         <v>75</v>
       </c>
@@ -8478,7 +8480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="424" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A424" s="1" t="s">
         <v>75</v>
       </c>
@@ -8495,7 +8497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A425" s="3" t="s">
         <v>75</v>
       </c>
@@ -8512,7 +8514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A426" s="1" t="s">
         <v>76</v>
       </c>
@@ -8529,7 +8531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="427" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A427" s="3" t="s">
         <v>76</v>
       </c>
@@ -8546,7 +8548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="428" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A428" s="1" t="s">
         <v>76</v>
       </c>
@@ -8563,7 +8565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="429" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A429" s="3" t="s">
         <v>76</v>
       </c>
@@ -8580,7 +8582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="430" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A430" s="1" t="s">
         <v>76</v>
       </c>
@@ -8597,7 +8599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="431" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A431" s="3" t="s">
         <v>76</v>
       </c>
@@ -8614,7 +8616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="432" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A432" s="1" t="s">
         <v>76</v>
       </c>
@@ -8631,7 +8633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="433" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A433" s="3" t="s">
         <v>76</v>
       </c>
@@ -8648,7 +8650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="434" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A434" s="1" t="s">
         <v>77</v>
       </c>
@@ -8665,7 +8667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="435" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A435" s="3" t="s">
         <v>77</v>
       </c>
@@ -8682,7 +8684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="436" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A436" s="1" t="s">
         <v>77</v>
       </c>
@@ -8699,7 +8701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="437" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A437" s="3" t="s">
         <v>77</v>
       </c>
@@ -8716,7 +8718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="438" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A438" s="1" t="s">
         <v>77</v>
       </c>
@@ -8733,7 +8735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="439" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A439" s="3" t="s">
         <v>77</v>
       </c>
@@ -8750,7 +8752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="440" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A440" s="1" t="s">
         <v>77</v>
       </c>
@@ -8767,7 +8769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="441" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A441" s="3" t="s">
         <v>77</v>
       </c>
@@ -8784,7 +8786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="442" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A442" s="1" t="s">
         <v>78</v>
       </c>
@@ -8801,7 +8803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="443" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A443" s="3" t="s">
         <v>78</v>
       </c>
@@ -8818,7 +8820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="444" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A444" s="1" t="s">
         <v>78</v>
       </c>
@@ -8835,7 +8837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="445" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A445" s="3" t="s">
         <v>78</v>
       </c>
@@ -8852,7 +8854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="446" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A446" s="1" t="s">
         <v>78</v>
       </c>
@@ -8869,7 +8871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="447" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A447" s="3" t="s">
         <v>78</v>
       </c>
@@ -8886,7 +8888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="448" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A448" s="1" t="s">
         <v>78</v>
       </c>
@@ -8903,7 +8905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A449" s="3" t="s">
         <v>78</v>
       </c>
@@ -8920,7 +8922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="450" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A450" s="1" t="s">
         <v>79</v>
       </c>
@@ -8937,7 +8939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A451" s="3" t="s">
         <v>79</v>
       </c>
@@ -8954,7 +8956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="452" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
         <v>79</v>
       </c>
@@ -8971,7 +8973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="453" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A453" s="3" t="s">
         <v>79</v>
       </c>
@@ -8988,7 +8990,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="454" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A454" s="1" t="s">
         <v>79</v>
       </c>
@@ -9005,7 +9007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="455" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A455" s="3" t="s">
         <v>79</v>
       </c>
@@ -9022,7 +9024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="456" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A456" s="1" t="s">
         <v>79</v>
       </c>
@@ -9039,7 +9041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="457" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A457" s="3" t="s">
         <v>79</v>
       </c>
@@ -9056,7 +9058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A458" s="1" t="s">
         <v>80</v>
       </c>
@@ -9073,7 +9075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="459" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A459" s="3" t="s">
         <v>80</v>
       </c>
@@ -9090,7 +9092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="460" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A460" s="1" t="s">
         <v>80</v>
       </c>
@@ -9107,7 +9109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="461" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A461" s="3" t="s">
         <v>80</v>
       </c>
@@ -9124,7 +9126,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="462" spans="1:5" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:5" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A462" s="1" t="s">
         <v>80</v>
       </c>
@@ -9141,7 +9143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="463" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A463" s="3" t="s">
         <v>80</v>
       </c>
@@ -9158,7 +9160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="464" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A464" s="1" t="s">
         <v>80</v>
       </c>
@@ -9175,7 +9177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="465" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A465" s="3" t="s">
         <v>80</v>
       </c>
@@ -9192,7 +9194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="466" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A466" s="1" t="s">
         <v>81</v>
       </c>
@@ -9209,7 +9211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="467" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A467" s="3" t="s">
         <v>81</v>
       </c>
@@ -9226,7 +9228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="468" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A468" s="1" t="s">
         <v>81</v>
       </c>
@@ -9243,7 +9245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="469" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A469" s="3" t="s">
         <v>81</v>
       </c>
@@ -9260,7 +9262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="470" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A470" s="1" t="s">
         <v>81</v>
       </c>
@@ -9277,7 +9279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="471" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A471" s="3" t="s">
         <v>81</v>
       </c>
@@ -9294,7 +9296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="472" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A472" s="1" t="s">
         <v>81</v>
       </c>
@@ -9311,7 +9313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="473" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A473" s="3" t="s">
         <v>81</v>
       </c>
@@ -9328,45 +9330,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="474" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>